<commit_message>
feat: Implementeer hoofd- en subcategorieën
</commit_message>
<xml_diff>
--- a/public/opdrachten.xlsx
+++ b/public/opdrachten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Fruitautomaat\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Fruitautomaat-R2P\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F72DF38-5D68-410D-B3DE-C963634B320E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1C7B4F-4255-44A3-840C-2C6B765E8D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opdrachten" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Categorie</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>Extra_Punten (max 2)</t>
+  </si>
+  <si>
+    <t>Hoofdcategorie</t>
+  </si>
+  <si>
+    <t>enkel</t>
+  </si>
+  <si>
+    <t>voet</t>
+  </si>
+  <si>
+    <t>knie</t>
   </si>
 </sst>
 </file>
@@ -514,198 +526,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>20</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="91.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>20</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="91.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>30</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>15</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="112.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" ht="112.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>15</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="112.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" ht="112.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="91.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>15</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>25</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="132.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:6" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>15</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="163.19999999999999" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:6" ht="163.19999999999999" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>25</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Implementeer geavanceerd filtersysteem
Voegt een geavanceerd filtersysteem toe voor opdrachten, inclusief filteren op bron en type. Belangrijkste wijzigingen:

- **src/data/types.ts & useOpdrachten.ts**: Datalaag uitgebreid met 'opdrachtType'.
- **src/components/FilterDashboard.tsx**: Nieuw component met klikbare icoontjes in het linkermenu voor directe filtercontrole.
- **src/components/CriteriaModal.tsx**: Nieuwe popup met gedetailleerde tabel van opdrachten per categorie en type.
- **src/App.tsx**: Centrale state management voor filters, inclusief persistentie in localStorage.
- **src/components/Fruitautomaat.tsx**: Visuele feedback met icoontjes voor bron en type opdracht.
- Tellers in UI geüpdatet om rekening te houden met actieve filters.
</commit_message>
<xml_diff>
--- a/public/opdrachten.xlsx
+++ b/public/opdrachten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Fruitautomaat-R2P\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C39646-53BD-4A28-9BEE-280C07853C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545CB20E-DBE2-4B31-A4F2-F6F25CF615FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opdrachten" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Hoofdcategorie</t>
   </si>
@@ -149,6 +149,72 @@
   </si>
   <si>
     <t>Humerus</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test vraag</t>
+  </si>
+  <si>
+    <t>OpdrachtType</t>
+  </si>
+  <si>
+    <t>feitenkennis</t>
+  </si>
+  <si>
+    <t>toepassing</t>
+  </si>
+  <si>
+    <t>Feitenkennis</t>
+  </si>
+  <si>
+    <t>Wat zijn de drie fases van weefselherstel?</t>
+  </si>
+  <si>
+    <t>Waarom is de ontstekingsfase belangrijk voor genezing?</t>
+  </si>
+  <si>
+    <t>Begrijpen</t>
+  </si>
+  <si>
+    <t>Demonstreer een effectieve oefening voor het versterken van de quadriceps.</t>
+  </si>
+  <si>
+    <t>Toepassing</t>
+  </si>
+  <si>
+    <t>Praktijk</t>
+  </si>
+  <si>
+    <t>Fysiotherapie</t>
+  </si>
+  <si>
+    <t>Communicatie</t>
+  </si>
+  <si>
+    <t>Tekenen</t>
+  </si>
+  <si>
+    <t>Uitleggen</t>
+  </si>
+  <si>
+    <t>Leg aan een patiënt uit wat het verschil is tussen artritis en artrose.</t>
+  </si>
+  <si>
+    <t>Teken de anatomie van het kniegewricht, inclusief de kruisbanden en menisci.</t>
+  </si>
+  <si>
+    <t>Voer een rollenspel uit waarin je een patiënt motiveert om zijn thuisoefeningen te doen.</t>
+  </si>
+  <si>
+    <t>Welke manuele techniek zou je toepassen bij een patiënt met een tenniselleboog?</t>
+  </si>
+  <si>
+    <t>Analyseer deze (fictieve) casus en stel een behandelplan op voor de eerste twee weken.</t>
+  </si>
+  <si>
+    <t>wel</t>
   </si>
 </sst>
 </file>
@@ -525,15 +591,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.09765625" customWidth="1"/>
+    <col min="4" max="4" width="68.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.09765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,19 +616,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -561,19 +639,22 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -581,19 +662,22 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>45</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -601,19 +685,22 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>20</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -621,19 +708,22 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>25</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -641,19 +731,22 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>25</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -661,19 +754,22 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -681,19 +777,22 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>15</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -701,19 +800,22 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>40</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -721,19 +823,22 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>35</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -741,19 +846,22 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>60</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -761,22 +869,124 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>40</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>30</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A7:F12 A1:F5" numberStoredAsText="1"/>
+    <ignoredError sqref="D7:G12 D1:G5 A1:B5 A7:B12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>